<commit_message>
new bussystem minor imrovements
Now also plots congestion before CBC (Colorblind friendly), also going to add more extensive messaging for when case is not balanceable, and why
</commit_message>
<xml_diff>
--- a/3_bus_input.xlsx
+++ b/3_bus_input.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://tenneteu-my.sharepoint.com/personal/joep_van_schelven_tennet_eu/Documents/Thesis/Werkdocumenten/Model/Model/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\304723\Documents\GitHub\CBC_RD_thesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="308" documentId="8_{EEA84B42-9857-4392-94EC-252B65C90BB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A19039D1-BE11-4ACA-9CCB-B5FE0E357102}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B46EE3-C030-4A24-9778-72A96BD46D2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="13710" windowWidth="38700" windowHeight="15435" activeTab="6" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="2" xr2:uid="{4D1B5A0D-1CEB-45D9-8796-95763D14CA6B}"/>
   </bookViews>
   <sheets>
     <sheet name="title_page" sheetId="1" r:id="rId1"/>
@@ -232,10 +232,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -541,17 +537,17 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -559,7 +555,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -567,7 +563,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -586,9 +582,9 @@
       <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -605,7 +601,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -622,7 +618,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -639,7 +635,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -665,18 +661,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F09800-6293-4D04-974E-A2660D60FC26}">
   <dimension ref="A1:Z10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:Z8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="6.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -756,7 +752,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -836,7 +832,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -916,7 +912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -954,7 +950,7 @@
         <v>105</v>
       </c>
       <c r="M4">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="N4">
         <v>105</v>
@@ -996,23 +992,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
     </row>
@@ -1029,17 +1025,17 @@
       <selection activeCell="D4" sqref="D4:Z4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="12" width="3.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="17" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="26" width="3.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="3.54296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="26" width="3.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -1119,7 +1115,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1199,11 +1195,11 @@
         <v>-10</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
     </row>
@@ -1220,14 +1216,14 @@
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="4.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -1261,7 +1257,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1272,7 +1268,7 @@
         <v>-100</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1283,7 +1279,7 @@
         <v>-400</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:26" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1299,18 +1295,18 @@
       <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
     </row>
   </sheetData>
@@ -1322,24 +1318,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50A915C1-4CB9-4DD7-B6E4-10F8FAF3EAA1}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.81640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.7109375" style="3"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>11</v>
       </c>
@@ -1359,7 +1355,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -1382,7 +1378,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -1405,7 +1401,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -1428,7 +1424,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>

</xml_diff>